<commit_message>
new variables, new issues, new resolves...
</commit_message>
<xml_diff>
--- a/assets/My_readings.xlsx
+++ b/assets/My_readings.xlsx
@@ -308,8 +308,8 @@
   </sheetPr>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -364,10 +364,10 @@
         <v>43954</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0</v>
+        <v>0.65625</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -396,10 +396,10 @@
         <v>43899</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -428,10 +428,10 @@
         <v>43901</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0</v>
+        <v>0.791666666666667</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
@@ -460,10 +460,10 @@
         <v>43901</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0</v>
+        <v>0.840277777777778</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0</v>
+        <v>0.861111111111111</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>13</v>
@@ -492,10 +492,10 @@
         <v>43912</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0</v>
+        <v>0.791666666666667</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
@@ -524,10 +524,10 @@
         <v>43917</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0</v>
+        <v>0.791666666666667</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>13</v>
@@ -556,10 +556,10 @@
         <v>43921</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0</v>
+        <v>0.604166666666667</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -588,10 +588,10 @@
         <v>43933</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0</v>
+        <v>0.694444444444444</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>13</v>
@@ -620,10 +620,10 @@
         <v>43969</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0</v>
+        <v>0.78125</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>13</v>
@@ -748,10 +748,10 @@
         <v>43975</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>0</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0</v>
+        <v>0.729166666666667</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>10</v>
@@ -780,10 +780,10 @@
         <v>43975</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>0</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0</v>
+        <v>0.854166666666667</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>16</v>
@@ -812,10 +812,10 @@
         <v>43976</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>0</v>
+        <v>0.791666666666667</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>10</v>
@@ -844,10 +844,10 @@
         <v>43976</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>0</v>
+        <v>0.836805555555556</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0</v>
+        <v>0.857638888888889</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>16</v>
@@ -876,10 +876,10 @@
         <v>43977</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0</v>
+        <v>0.763888888888889</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>10</v>
@@ -908,10 +908,10 @@
         <v>43977</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>0</v>
+        <v>0.770833333333333</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0</v>
+        <v>0.8125</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>16</v>
@@ -940,10 +940,10 @@
         <v>43986</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>16</v>
@@ -963,10 +963,10 @@
         <v>43987</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>0</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0</v>
+        <v>0.604166666666667</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>16</v>
@@ -986,10 +986,10 @@
         <v>43988</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>0</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0</v>
+        <v>0.729166666666667</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>16</v>
@@ -1009,10 +1009,10 @@
         <v>43990</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>0</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0</v>
+        <v>0.836805555555556</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>10</v>
@@ -1041,10 +1041,10 @@
         <v>43990</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>0</v>
+        <v>0.840277777777778</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0</v>
+        <v>0.881944444444444</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>19</v>
@@ -1073,10 +1073,10 @@
         <v>43991</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>0</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0</v>
+        <v>0.763888888888889</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>19</v>
@@ -1105,10 +1105,10 @@
         <v>43993</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>0</v>
+        <v>0.791666666666667</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>19</v>
@@ -1137,10 +1137,10 @@
         <v>43994</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>0</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>19</v>

</xml_diff>